<commit_message>
New Modification Asset manager
</commit_message>
<xml_diff>
--- a/TestData/Assetmanager.xlsx
+++ b/TestData/Assetmanager.xlsx
@@ -4,12 +4,14 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6800" activeTab="2"/>
+    <workbookView windowWidth="19200" windowHeight="6080" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Login" sheetId="3" r:id="rId1"/>
-    <sheet name="CompliancePolicy" sheetId="1" r:id="rId2"/>
-    <sheet name="ManageTask(TM)" sheetId="2" r:id="rId3"/>
+    <sheet name="AssetMaster" sheetId="4" r:id="rId1"/>
+    <sheet name="AssetAllocation" sheetId="5" r:id="rId2"/>
+    <sheet name="AssetMovement" sheetId="6" r:id="rId3"/>
+    <sheet name="CompliancePolicy" sheetId="1" r:id="rId4"/>
+    <sheet name="ManageTask(TM)" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +31,202 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="120">
+  <si>
+    <t>AssetID</t>
+  </si>
+  <si>
+    <t>AssetName</t>
+  </si>
+  <si>
+    <t>AssetCode</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>PurchaseAmount</t>
+  </si>
+  <si>
+    <t>Pur_date</t>
+  </si>
+  <si>
+    <t>Pur_month</t>
+  </si>
+  <si>
+    <t>Pur_year</t>
+  </si>
+  <si>
+    <t>ImagePath</t>
+  </si>
+  <si>
+    <t>WaterBottle</t>
+  </si>
+  <si>
+    <t>WB-01</t>
+  </si>
+  <si>
+    <t>Other Materials</t>
+  </si>
+  <si>
+    <t>Aug</t>
+  </si>
+  <si>
+    <t>C:/Users/PradeepElumalai/OneDrive - Medyaan Healthcare Private Limited/Pictures/leop.jpg</t>
+  </si>
+  <si>
+    <t>TorchLight</t>
+  </si>
+  <si>
+    <t>Unknown Materials</t>
+  </si>
+  <si>
+    <t>Sep</t>
+  </si>
+  <si>
+    <t>C:\Users\PradeepElumalai\OneDrive - Medyaan Healthcare Private Limited\Pictures\key5.jpg</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>RoomType</t>
+  </si>
+  <si>
+    <t>Room</t>
+  </si>
+  <si>
+    <t>AllocationPurpose</t>
+  </si>
+  <si>
+    <t>Startdate</t>
+  </si>
+  <si>
+    <t>Startmonth</t>
+  </si>
+  <si>
+    <t>Startyear</t>
+  </si>
+  <si>
+    <t>Enddate</t>
+  </si>
+  <si>
+    <t>Endmonth</t>
+  </si>
+  <si>
+    <t>Endyear</t>
+  </si>
+  <si>
+    <t>Filter</t>
+  </si>
+  <si>
+    <t>Ej</t>
+  </si>
+  <si>
+    <t>Forceps</t>
+  </si>
+  <si>
+    <t>Room Type</t>
+  </si>
+  <si>
+    <t>sample1234</t>
+  </si>
+  <si>
+    <t>General Use</t>
+  </si>
+  <si>
+    <t>Ej Pradeep</t>
+  </si>
+  <si>
+    <t>MovementType</t>
+  </si>
+  <si>
+    <t>TransferType</t>
+  </si>
+  <si>
+    <t>DestinationArea</t>
+  </si>
+  <si>
+    <t>DestinationRoomType</t>
+  </si>
+  <si>
+    <t>DestinationRoom</t>
+  </si>
+  <si>
+    <t>ExternalDestination</t>
+  </si>
+  <si>
+    <t>ReturnDate</t>
+  </si>
+  <si>
+    <t>ReturnMonth</t>
+  </si>
+  <si>
+    <t>ReturnYear</t>
+  </si>
+  <si>
+    <t>Purpose</t>
+  </si>
+  <si>
+    <t>GatePass</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>CreatedDate</t>
+  </si>
+  <si>
+    <t>Reason</t>
+  </si>
+  <si>
+    <t>External</t>
+  </si>
+  <si>
+    <t>Temporary</t>
+  </si>
+  <si>
+    <t>Cattery</t>
+  </si>
+  <si>
+    <t>B6 (Cat)</t>
+  </si>
+  <si>
+    <t>Cat Holding</t>
+  </si>
+  <si>
+    <t>Create 7(Cat)</t>
+  </si>
+  <si>
+    <t>Near Canada</t>
+  </si>
+  <si>
+    <t>Nov</t>
+  </si>
+  <si>
+    <t>Reallocation</t>
+  </si>
+  <si>
+    <t>Auto Test 069</t>
+  </si>
+  <si>
+    <t>Automation Purpose</t>
+  </si>
+  <si>
+    <t>Internal</t>
+  </si>
+  <si>
+    <t>Permanent</t>
+  </si>
+  <si>
+    <t>Crate 7 (Cat)</t>
+  </si>
+  <si>
+    <t>ET-02</t>
+  </si>
   <si>
     <t>taskname</t>
   </si>
@@ -97,18 +294,12 @@
     <t>weekend</t>
   </si>
   <si>
-    <t>Sep</t>
-  </si>
-  <si>
     <t>30</t>
   </si>
   <si>
     <t>this Compliance Policy was created by using Automation</t>
   </si>
   <si>
-    <t>Filter</t>
-  </si>
-  <si>
     <t>Search</t>
   </si>
   <si>
@@ -155,9 +346,6 @@
   </si>
   <si>
     <t>Note</t>
-  </si>
-  <si>
-    <t>ImagePath</t>
   </si>
   <si>
     <t>TaskTab</t>
@@ -215,7 +403,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -265,6 +453,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -744,137 +940,137 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -936,6 +1132,18 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1278,20 +1486,462 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14" outlineLevelRow="2"/>
+  <cols>
+    <col min="1" max="1" width="11.25" style="27"/>
+    <col min="2" max="2" width="11.25" style="27" customWidth="1"/>
+    <col min="3" max="3" width="9.75" style="27" customWidth="1"/>
+    <col min="4" max="5" width="14.9166666666667" style="27" customWidth="1"/>
+    <col min="6" max="6" width="13" style="27" customWidth="1"/>
+    <col min="7" max="7" width="9.66666666666667" style="27" customWidth="1"/>
+    <col min="8" max="8" width="11.75" style="27" customWidth="1"/>
+    <col min="9" max="16384" width="36.8333333333333" style="27"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="26" customFormat="1" spans="1:9">
+      <c r="A1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" ht="27" customHeight="1" spans="2:9">
+      <c r="B2" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="27">
+        <v>100</v>
+      </c>
+      <c r="F2" s="27">
+        <v>21</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="27">
+        <v>2025</v>
+      </c>
+      <c r="I2" s="28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9">
+      <c r="B3" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="27">
+        <v>1500</v>
+      </c>
+      <c r="F3" s="27">
+        <v>10</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="27">
+        <v>2023</v>
+      </c>
+      <c r="I3" s="27" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:O3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14" outlineLevelRow="2"/>
+  <cols>
+    <col min="1" max="1" width="11.0833333333333" customWidth="1"/>
+    <col min="3" max="4" width="10.1666666666667" customWidth="1"/>
+    <col min="5" max="5" width="12.75" customWidth="1"/>
+    <col min="7" max="7" width="15.6666666666667" customWidth="1"/>
+    <col min="8" max="8" width="10.0833333333333" customWidth="1"/>
+    <col min="9" max="9" width="10.4166666666667" customWidth="1"/>
+    <col min="10" max="11" width="9.83333333333333" customWidth="1"/>
+    <col min="14" max="14" width="1.25" style="24" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2">
+        <v>2026</v>
+      </c>
+      <c r="K2">
+        <v>12</v>
+      </c>
+      <c r="L2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2">
+        <v>2027</v>
+      </c>
+      <c r="O2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" customFormat="1" spans="1:15">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3">
+        <v>12</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3">
+        <v>2026</v>
+      </c>
+      <c r="K3">
+        <v>12</v>
+      </c>
+      <c r="L3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3">
+        <v>2027</v>
+      </c>
+      <c r="N3" s="24"/>
+      <c r="O3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:T4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="T8" sqref="T8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14" outlineLevelRow="3"/>
+  <cols>
+    <col min="1" max="1" width="10.5833333333333" customWidth="1"/>
+    <col min="2" max="2" width="14.0833333333333" customWidth="1"/>
+    <col min="3" max="3" width="14.3333333333333" customWidth="1"/>
+    <col min="4" max="4" width="7.58333333333333" customWidth="1"/>
+    <col min="5" max="5" width="10.5" customWidth="1"/>
+    <col min="7" max="7" width="15.0833333333333" customWidth="1"/>
+    <col min="8" max="8" width="18.3333333333333" customWidth="1"/>
+    <col min="9" max="9" width="14.8333333333333" customWidth="1"/>
+    <col min="10" max="10" width="17" customWidth="1"/>
+    <col min="11" max="11" width="11.25" customWidth="1"/>
+    <col min="12" max="12" width="11.9166666666667" customWidth="1"/>
+    <col min="13" max="13" width="10" customWidth="1"/>
+    <col min="14" max="14" width="12.8333333333333" customWidth="1"/>
+    <col min="15" max="15" width="11.8333333333333" customWidth="1"/>
+    <col min="16" max="16" width="1.75" style="24" customWidth="1"/>
+    <col min="17" max="17" width="10.0833333333333" customWidth="1"/>
+    <col min="18" max="18" width="9.91666666666667" customWidth="1"/>
+    <col min="19" max="19" width="10.8333333333333" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="23" customFormat="1" spans="1:20">
+      <c r="A1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="N1" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O1" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="R1" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="S1" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="T1" s="23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
+      <c r="A2">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K2">
+        <v>14</v>
+      </c>
+      <c r="L2" t="s">
+        <v>57</v>
+      </c>
+      <c r="M2">
+        <v>2025</v>
+      </c>
+      <c r="N2" t="s">
+        <v>58</v>
+      </c>
+      <c r="O2" t="s">
+        <v>59</v>
+      </c>
+      <c r="T2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J3" t="s">
+        <v>56</v>
+      </c>
+      <c r="K3">
+        <v>14</v>
+      </c>
+      <c r="L3" t="s">
+        <v>57</v>
+      </c>
+      <c r="M3">
+        <v>2025</v>
+      </c>
+      <c r="N3" t="s">
+        <v>58</v>
+      </c>
+      <c r="O3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="17:20">
+      <c r="Q4" t="s">
+        <v>35</v>
+      </c>
+      <c r="R4" t="s">
+        <v>64</v>
+      </c>
+      <c r="T4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:O4"/>
@@ -1319,96 +1969,96 @@
   <sheetData>
     <row r="1" s="17" customFormat="1" spans="1:15">
       <c r="A1" s="14" t="s">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>1</v>
+        <v>66</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>2</v>
+        <v>67</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>3</v>
+        <v>68</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>4</v>
+        <v>69</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>5</v>
+        <v>70</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>6</v>
+        <v>71</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>7</v>
+        <v>72</v>
       </c>
       <c r="I1" s="17" t="s">
-        <v>8</v>
+        <v>73</v>
       </c>
       <c r="J1" s="17" t="s">
-        <v>9</v>
+        <v>74</v>
       </c>
       <c r="K1" s="17" t="s">
-        <v>10</v>
+        <v>75</v>
       </c>
       <c r="L1" s="14" t="s">
-        <v>11</v>
+        <v>76</v>
       </c>
       <c r="M1" s="17" t="s">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="N1" s="17" t="s">
-        <v>13</v>
+        <v>78</v>
       </c>
       <c r="O1" s="14" t="s">
-        <v>14</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" s="18" customFormat="1" ht="29" customHeight="1" spans="1:15">
       <c r="A2" s="18" t="s">
-        <v>15</v>
+        <v>80</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>16</v>
+        <v>81</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>17</v>
+        <v>82</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>18</v>
+        <v>83</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>20</v>
+        <v>85</v>
       </c>
       <c r="G2" s="18">
         <v>10</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>21</v>
+        <v>86</v>
       </c>
       <c r="I2" s="18">
         <v>20</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K2" s="18">
         <v>2025</v>
       </c>
       <c r="L2" s="18" t="s">
-        <v>23</v>
+        <v>87</v>
       </c>
       <c r="M2" s="18" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="N2" s="18">
         <v>2030</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>24</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="5:5">
@@ -1420,13 +2070,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:X5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="T14" sqref="T14"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R1" sqref="$A1:$XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.1666666666667" defaultRowHeight="14" outlineLevelRow="4"/>
@@ -1449,87 +2099,87 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="31" spans="1:24">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>26</v>
+        <v>89</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="5" t="s">
-        <v>27</v>
+        <v>90</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>28</v>
+        <v>91</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>29</v>
+        <v>92</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>30</v>
+        <v>93</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>31</v>
+        <v>94</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>32</v>
+        <v>95</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>33</v>
+        <v>96</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>34</v>
+        <v>97</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>35</v>
+        <v>98</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>36</v>
+        <v>99</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>37</v>
+        <v>100</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>38</v>
+        <v>101</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="Q1" s="11"/>
       <c r="R1" s="12" t="s">
-        <v>40</v>
+        <v>103</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>41</v>
+        <v>104</v>
       </c>
       <c r="T1" s="5" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="U1" s="13" t="s">
-        <v>43</v>
+        <v>105</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>44</v>
+        <v>106</v>
       </c>
       <c r="W1" s="14" t="s">
-        <v>45</v>
+        <v>107</v>
       </c>
       <c r="X1" s="14" t="s">
-        <v>46</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" s="2" customFormat="1" spans="1:24">
       <c r="A2" s="2" t="s">
-        <v>47</v>
+        <v>109</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>48</v>
+        <v>110</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="8" t="s">
-        <v>49</v>
+        <v>111</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>16</v>
+        <v>81</v>
       </c>
       <c r="F2" s="8">
         <v>1</v>
@@ -1541,7 +2191,7 @@
         <v>21</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="J2" s="8">
         <v>2025</v>
@@ -1549,39 +2199,39 @@
       <c r="K2" s="10">
         <v>0.416666666666667</v>
       </c>
-      <c r="L2" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="M2" s="23" t="s">
-        <v>51</v>
+      <c r="L2" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="M2" s="29" t="s">
+        <v>113</v>
       </c>
       <c r="N2" s="8">
         <v>17</v>
       </c>
-      <c r="O2" s="23" t="s">
-        <v>51</v>
+      <c r="O2" s="29" t="s">
+        <v>113</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>52</v>
+        <v>114</v>
       </c>
       <c r="Q2" s="15"/>
       <c r="R2" s="2" t="s">
-        <v>16</v>
+        <v>81</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>53</v>
+        <v>115</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>54</v>
+        <v>116</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>55</v>
+        <v>117</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>56</v>
+        <v>118</v>
       </c>
       <c r="W2" s="16" t="s">
-        <v>57</v>
+        <v>119</v>
       </c>
       <c r="X2" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
Change Asset policy async methods
</commit_message>
<xml_diff>
--- a/TestData/Assetmanager.xlsx
+++ b/TestData/Assetmanager.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6200" firstSheet="2" activeTab="4"/>
+    <workbookView windowWidth="19200" windowHeight="6800" tabRatio="760" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="AssetMaster" sheetId="4" r:id="rId1"/>
@@ -12,8 +12,9 @@
     <sheet name="AssetMovement" sheetId="6" r:id="rId3"/>
     <sheet name="AssetDisposal" sheetId="7" r:id="rId4"/>
     <sheet name="AssetCategory" sheetId="8" r:id="rId5"/>
-    <sheet name="CompliancePolicy" sheetId="1" r:id="rId6"/>
-    <sheet name="ManageTask(TM)" sheetId="2" r:id="rId7"/>
+    <sheet name="AssetPolicy" sheetId="9" r:id="rId6"/>
+    <sheet name="CompliancePolicy" sheetId="1" r:id="rId7"/>
+    <sheet name="ManageTask(TM)" sheetId="2" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="189">
   <si>
     <t>AssetID</t>
   </si>
@@ -143,6 +144,9 @@
     <t>Ej Pradeep</t>
   </si>
   <si>
+    <t>Nov</t>
+  </si>
+  <si>
     <t>MovementType</t>
   </si>
   <si>
@@ -206,9 +210,6 @@
     <t>Near Canada</t>
   </si>
   <si>
-    <t>Nov</t>
-  </si>
-  <si>
     <t>Reallocation</t>
   </si>
   <si>
@@ -296,75 +297,222 @@
     <t>Test Automation 7</t>
   </si>
   <si>
-    <t>taskname</t>
-  </si>
-  <si>
-    <t>project</t>
-  </si>
-  <si>
-    <t>auditrequired</t>
-  </si>
-  <si>
-    <t>assetname</t>
-  </si>
-  <si>
-    <t>Plannedhours</t>
-  </si>
-  <si>
-    <t>starttime1</t>
-  </si>
-  <si>
-    <t>starttime2</t>
-  </si>
-  <si>
-    <t>recurrence</t>
-  </si>
-  <si>
-    <t>startDate</t>
-  </si>
-  <si>
-    <t>startMonth</t>
-  </si>
-  <si>
-    <t>startYear</t>
-  </si>
-  <si>
-    <t>endDate</t>
-  </si>
-  <si>
-    <t>endMonth</t>
-  </si>
-  <si>
-    <t>endYear</t>
-  </si>
-  <si>
-    <t>description</t>
+    <t>Taskname</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>AuditRequired</t>
+  </si>
+  <si>
+    <t>PlannedHours</t>
+  </si>
+  <si>
+    <t>StartHrs</t>
+  </si>
+  <si>
+    <t>StartMins</t>
+  </si>
+  <si>
+    <t>EndHrs</t>
+  </si>
+  <si>
+    <t>EndMins</t>
+  </si>
+  <si>
+    <t>Recurrence</t>
+  </si>
+  <si>
+    <t>StartDate</t>
+  </si>
+  <si>
+    <t>StartMonth</t>
+  </si>
+  <si>
+    <t>StartYear</t>
+  </si>
+  <si>
+    <t>EndDate</t>
+  </si>
+  <si>
+    <t>EndMonth</t>
+  </si>
+  <si>
+    <t>EndYear</t>
+  </si>
+  <si>
+    <t>FortNight1</t>
+  </si>
+  <si>
+    <t>FortNight2</t>
+  </si>
+  <si>
+    <t>Week</t>
+  </si>
+  <si>
+    <t>Month_date</t>
+  </si>
+  <si>
+    <t>Year_month</t>
+  </si>
+  <si>
+    <t>Year_date</t>
+  </si>
+  <si>
+    <t>Automation Policy-01</t>
+  </si>
+  <si>
+    <t>TestProject</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>Weekday</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>2026</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>2027</t>
+  </si>
+  <si>
+    <t>Automation Policy-02</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>Weekend</t>
+  </si>
+  <si>
+    <t>Automation Policy-03</t>
+  </si>
+  <si>
+    <t>Asset Policy Request</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Fortnight</t>
+  </si>
+  <si>
+    <t>Dec</t>
+  </si>
+  <si>
+    <t>Monday','Tuesday','Wednesday'</t>
+  </si>
+  <si>
+    <t>Monday','Wednesday','Tuesday','Thursday','Friday','Sunday'</t>
+  </si>
+  <si>
+    <t>Automation Policy-04</t>
+  </si>
+  <si>
+    <t>(9)</t>
+  </si>
+  <si>
+    <t>02:25</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>2025</t>
+  </si>
+  <si>
+    <t>Automation Policy-05</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>monthly</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>Mar</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Automation Policy-06</t>
+  </si>
+  <si>
+    <t>(8)</t>
+  </si>
+  <si>
+    <t>03:20</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>Yearly</t>
+  </si>
+  <si>
+    <t>Apr</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Starttime1</t>
+  </si>
+  <si>
+    <t>Starttime2</t>
   </si>
   <si>
     <t>Automation Compliance Policy - 02</t>
   </si>
   <si>
-    <t>TestProject</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>Phone</t>
   </si>
   <si>
     <t>00:15</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
     <t>weekend</t>
   </si>
   <si>
-    <t>30</t>
-  </si>
-  <si>
     <t>this Compliance Policy was created by using Automation</t>
   </si>
   <si>
@@ -372,9 +520,6 @@
   </si>
   <si>
     <t>TaskTitle</t>
-  </si>
-  <si>
-    <t>Project</t>
   </si>
   <si>
     <t>Priority</t>
@@ -468,7 +613,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -516,6 +661,14 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
@@ -1005,137 +1158,137 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1197,17 +1350,41 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" quotePrefix="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" quotePrefix="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1559,91 +1736,91 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="1" width="11.25" style="27"/>
-    <col min="2" max="2" width="11.25" style="27" customWidth="1"/>
-    <col min="3" max="3" width="9.75" style="27" customWidth="1"/>
-    <col min="4" max="5" width="14.9166666666667" style="27" customWidth="1"/>
-    <col min="6" max="6" width="13" style="27" customWidth="1"/>
-    <col min="7" max="7" width="9.66666666666667" style="27" customWidth="1"/>
-    <col min="8" max="8" width="11.75" style="27" customWidth="1"/>
-    <col min="9" max="16384" width="36.8333333333333" style="27"/>
+    <col min="1" max="1" width="11.25" style="33"/>
+    <col min="2" max="2" width="11.25" style="33" customWidth="1"/>
+    <col min="3" max="3" width="9.75" style="33" customWidth="1"/>
+    <col min="4" max="5" width="14.9166666666667" style="33" customWidth="1"/>
+    <col min="6" max="6" width="13" style="33" customWidth="1"/>
+    <col min="7" max="7" width="9.66666666666667" style="33" customWidth="1"/>
+    <col min="8" max="8" width="11.75" style="33" customWidth="1"/>
+    <col min="9" max="16384" width="36.8333333333333" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" s="24" customFormat="1" spans="1:9">
-      <c r="A1" s="24" t="s">
+    <row r="1" s="30" customFormat="1" spans="1:9">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="I1" s="30" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" ht="27" customHeight="1" spans="2:9">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="27">
+      <c r="E2" s="33">
         <v>100</v>
       </c>
-      <c r="F2" s="27">
+      <c r="F2" s="33">
         <v>21</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="27">
+      <c r="H2" s="33">
         <v>2025</v>
       </c>
-      <c r="I2" s="28" t="s">
+      <c r="I2" s="34" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="2:9">
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="27">
+      <c r="E3" s="33">
         <v>1500</v>
       </c>
-      <c r="F3" s="27">
+      <c r="F3" s="33">
         <v>10</v>
       </c>
-      <c r="G3" s="27" t="s">
+      <c r="G3" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="27">
+      <c r="H3" s="33">
         <v>2023</v>
       </c>
-      <c r="I3" s="27" t="s">
+      <c r="I3" s="33" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1656,13 +1833,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14" outlineLevelRow="3"/>
   <cols>
     <col min="1" max="1" width="11.0833333333333" customWidth="1"/>
     <col min="3" max="4" width="10.1666666666667" customWidth="1"/>
@@ -1671,7 +1848,7 @@
     <col min="8" max="8" width="10.0833333333333" customWidth="1"/>
     <col min="9" max="9" width="10.4166666666667" customWidth="1"/>
     <col min="10" max="11" width="9.83333333333333" customWidth="1"/>
-    <col min="14" max="14" width="1.25" style="25" customWidth="1"/>
+    <col min="14" max="14" width="1.25" style="31" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -1790,14 +1967,28 @@
       <c r="M3">
         <v>2027</v>
       </c>
-      <c r="N3" s="25"/>
+      <c r="N3" s="31"/>
       <c r="O3" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="8:10">
+      <c r="H4">
+        <v>7</v>
+      </c>
+      <c r="I4" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4">
+        <v>2026</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
+  <ignoredErrors>
+    <ignoredError sqref="A1:O2 A3:G4 I3:O4" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -1826,70 +2017,70 @@
     <col min="13" max="13" width="10" customWidth="1"/>
     <col min="14" max="14" width="12.8333333333333" customWidth="1"/>
     <col min="15" max="15" width="11.8333333333333" customWidth="1"/>
-    <col min="16" max="16" width="1.75" style="25" customWidth="1"/>
+    <col min="16" max="16" width="1.75" style="31" customWidth="1"/>
     <col min="17" max="17" width="10.0833333333333" customWidth="1"/>
     <col min="18" max="18" width="9.91666666666667" customWidth="1"/>
     <col min="19" max="19" width="10.8333333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="23" customFormat="1" spans="1:20">
-      <c r="A1" s="23" t="s">
+    <row r="1" s="29" customFormat="1" spans="1:20">
+      <c r="A1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="23" t="s">
+      <c r="B1" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="C1" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="H1" s="23" t="s">
+      <c r="G1" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="H1" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="I1" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="J1" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="L1" s="23" t="s">
+      <c r="K1" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="M1" s="23" t="s">
+      <c r="L1" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="N1" s="23" t="s">
+      <c r="M1" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="O1" s="23" t="s">
+      <c r="N1" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="23" t="s">
+      <c r="O1" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="R1" s="23" t="s">
+      <c r="P1" s="32"/>
+      <c r="Q1" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="R1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="S1" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="T1" s="23" t="s">
+      <c r="S1" s="29" t="s">
         <v>49</v>
+      </c>
+      <c r="T1" s="29" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -1897,37 +2088,37 @@
         <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G2" t="s">
         <v>21</v>
       </c>
       <c r="H2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K2">
         <v>14</v>
       </c>
       <c r="L2" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="M2">
         <v>2025</v>
@@ -1956,28 +2147,28 @@
         <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G3" t="s">
         <v>21</v>
       </c>
       <c r="H3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I3" t="s">
         <v>63</v>
       </c>
       <c r="J3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K3">
         <v>14</v>
       </c>
       <c r="L3" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="M3">
         <v>2025</v>
@@ -2008,7 +2199,7 @@
         <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -2032,39 +2223,39 @@
     <col min="2" max="2" width="15.1666666666667" customWidth="1"/>
     <col min="3" max="3" width="15.8333333333333" customWidth="1"/>
     <col min="4" max="4" width="17.4166666666667" customWidth="1"/>
-    <col min="9" max="9" width="1.40833333333333" style="25" customWidth="1"/>
+    <col min="9" max="9" width="1.40833333333333" style="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="24" customFormat="1" spans="1:11">
-      <c r="A1" s="24" t="s">
+    <row r="1" s="30" customFormat="1" spans="1:11">
+      <c r="A1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="H1" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="I1" s="26"/>
-      <c r="J1" s="24" t="s">
+      <c r="H1" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="32"/>
+      <c r="J1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="24" t="s">
+      <c r="K1" s="30" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2124,8 +2315,8 @@
   <sheetPr/>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14" outlineLevelRow="7" outlineLevelCol="1"/>
@@ -2133,11 +2324,11 @@
     <col min="1" max="1" width="16.9166666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="23" customFormat="1" spans="1:2">
-      <c r="A1" s="23" t="s">
+    <row r="1" s="29" customFormat="1" spans="1:2">
+      <c r="A1" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="29" t="s">
         <v>78</v>
       </c>
     </row>
@@ -2206,15 +2397,466 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
+  <dimension ref="A1:W7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14" outlineLevelRow="6"/>
+  <cols>
+    <col min="1" max="1" width="15.25" style="24" customWidth="1"/>
+    <col min="2" max="2" width="10.25" style="24" customWidth="1"/>
+    <col min="3" max="3" width="12.5833333333333" style="24" customWidth="1"/>
+    <col min="4" max="4" width="14" style="24" customWidth="1"/>
+    <col min="5" max="5" width="14.6666666666667" style="24" customWidth="1"/>
+    <col min="6" max="6" width="9.66666666666667" style="24" customWidth="1"/>
+    <col min="7" max="7" width="10.5833333333333" style="24" customWidth="1"/>
+    <col min="8" max="10" width="10.8333333333333" style="24" customWidth="1"/>
+    <col min="11" max="11" width="8.66666666666667" style="24"/>
+    <col min="12" max="12" width="11.4166666666667" style="24" customWidth="1"/>
+    <col min="13" max="14" width="8.66666666666667" style="24"/>
+    <col min="15" max="15" width="11.5833333333333" style="24" customWidth="1"/>
+    <col min="16" max="16" width="8.66666666666667" style="24"/>
+    <col min="17" max="17" width="20.1666666666667" style="24" customWidth="1"/>
+    <col min="18" max="18" width="15.8333333333333" style="24" customWidth="1"/>
+    <col min="19" max="19" width="15.3333333333333" style="24" customWidth="1"/>
+    <col min="20" max="20" width="17" style="24" customWidth="1"/>
+    <col min="21" max="21" width="12.9166666666667" style="24" customWidth="1"/>
+    <col min="22" max="22" width="12.3333333333333" style="24" customWidth="1"/>
+    <col min="23" max="23" width="9.91666666666667" style="24" customWidth="1"/>
+    <col min="24" max="16384" width="8.66666666666667" style="24"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="23" customFormat="1" spans="1:23">
+      <c r="A1" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="I1" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="J1" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="K1" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="L1" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="M1" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="N1" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="O1" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="P1" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q1" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="R1" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="S1" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="T1" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="U1" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="V1" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="W1" s="23" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" ht="28" spans="1:19">
+      <c r="A2" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="H2" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="I2" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="J2" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="K2" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="L2" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="N2" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="O2" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="P2" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q2" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="R2" s="24"/>
+      <c r="S2" s="28"/>
+    </row>
+    <row r="3" ht="28" spans="1:19">
+      <c r="A3" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="I3" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="J3" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="K3" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="L3" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="M3" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="N3" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="O3" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="P3" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q3" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="R3" s="24"/>
+      <c r="S3" s="28"/>
+    </row>
+    <row r="4" ht="56" spans="1:19">
+      <c r="A4" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="G4" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="H4" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="I4" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="J4" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="K4" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="L4" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="N4" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="O4" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="P4" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q4" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="R4" s="35" t="s">
+        <v>132</v>
+      </c>
+      <c r="S4" s="36" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" ht="28" spans="1:20">
+      <c r="A5" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="G5" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="H5" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="I5" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="J5" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="K5" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="L5" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="M5" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="N5" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="O5" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="P5" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q5" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="R5" s="24"/>
+      <c r="S5" s="28"/>
+      <c r="T5" s="35" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" ht="42" spans="1:21">
+      <c r="A6" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>140</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="F6" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="G6" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="H6" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="I6" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="J6" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="K6" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="L6" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="M6" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="N6" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="O6" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="P6" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q6" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="R6" s="24"/>
+      <c r="S6" s="28"/>
+      <c r="U6" s="24" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" ht="28" spans="1:23">
+      <c r="A7" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="F7" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="G7" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="H7" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="I7" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="J7" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="K7" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="L7" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="M7" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="N7" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="O7" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="P7" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q7" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="R7" s="24"/>
+      <c r="S7" s="28"/>
+      <c r="V7" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="W7" s="24" t="s">
+        <v>152</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A1" sqref="$A1:$XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="3"/>
   <cols>
-    <col min="1" max="3" width="28.75" style="19" customWidth="1"/>
+    <col min="1" max="1" width="29.0833333333333" style="19" customWidth="1"/>
+    <col min="2" max="3" width="28.75" style="19" customWidth="1"/>
     <col min="4" max="4" width="10.125" style="19" customWidth="1"/>
     <col min="5" max="5" width="14.375" style="19" customWidth="1"/>
     <col min="6" max="6" width="17.25" style="19" customWidth="1"/>
@@ -2222,14 +2864,14 @@
     <col min="9" max="9" width="9" style="19"/>
     <col min="10" max="10" width="12.6666666666667" style="19" customWidth="1"/>
     <col min="11" max="11" width="9.16666666666667" style="19" customWidth="1"/>
-    <col min="12" max="12" width="21.5" style="19" customWidth="1"/>
+    <col min="12" max="12" width="10.75" style="19" customWidth="1"/>
     <col min="13" max="13" width="12.6666666666667" style="19" customWidth="1"/>
     <col min="14" max="14" width="14.6666666666667" style="19" customWidth="1"/>
     <col min="15" max="15" width="23.9166666666667" style="19" customWidth="1"/>
     <col min="16" max="16384" width="9" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" s="17" customFormat="1" spans="1:15">
+    <row r="1" s="17" customFormat="1" ht="27" spans="1:15">
       <c r="A1" s="14" t="s">
         <v>87</v>
       </c>
@@ -2240,66 +2882,66 @@
         <v>89</v>
       </c>
       <c r="D1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="E1" s="14" t="s">
-        <v>91</v>
-      </c>
       <c r="F1" s="17" t="s">
-        <v>92</v>
+        <v>153</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>93</v>
+        <v>154</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I1" s="17" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J1" s="17" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="K1" s="17" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="L1" s="14" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="M1" s="17" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="N1" s="17" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="O1" s="14" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="2" s="18" customFormat="1" ht="29" customHeight="1" spans="1:15">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" s="18" customFormat="1" ht="19" customHeight="1" spans="1:15">
       <c r="A2" s="18" t="s">
-        <v>102</v>
+        <v>155</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>105</v>
+        <v>156</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>107</v>
+        <v>157</v>
+      </c>
+      <c r="F2" s="18">
+        <v>10</v>
       </c>
       <c r="G2" s="18">
         <v>10</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>108</v>
+        <v>158</v>
       </c>
       <c r="I2" s="18">
         <v>20</v>
@@ -2310,8 +2952,8 @@
       <c r="K2" s="18">
         <v>2025</v>
       </c>
-      <c r="L2" s="18" t="s">
-        <v>109</v>
+      <c r="L2" s="18">
+        <v>30</v>
       </c>
       <c r="M2" s="18" t="s">
         <v>16</v>
@@ -2320,7 +2962,7 @@
         <v>2030</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>110</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="5:5">
@@ -2332,7 +2974,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:X5"/>
@@ -2364,84 +3006,84 @@
         <v>29</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>111</v>
+        <v>160</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="5" t="s">
-        <v>112</v>
+        <v>161</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>114</v>
+        <v>162</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>115</v>
+        <v>163</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>116</v>
+        <v>164</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>117</v>
+        <v>165</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>118</v>
+        <v>166</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>119</v>
+        <v>167</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>120</v>
+        <v>168</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>121</v>
+        <v>169</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>122</v>
+        <v>170</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>123</v>
+        <v>171</v>
       </c>
       <c r="P1" s="5" t="s">
         <v>78</v>
       </c>
       <c r="Q1" s="11"/>
       <c r="R1" s="12" t="s">
-        <v>124</v>
+        <v>172</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>125</v>
+        <v>173</v>
       </c>
       <c r="T1" s="5" t="s">
         <v>8</v>
       </c>
       <c r="U1" s="13" t="s">
-        <v>126</v>
+        <v>174</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>127</v>
+        <v>175</v>
       </c>
       <c r="W1" s="14" t="s">
-        <v>128</v>
+        <v>176</v>
       </c>
       <c r="X1" s="14" t="s">
-        <v>129</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" s="2" customFormat="1" spans="1:24">
       <c r="A2" s="2" t="s">
-        <v>130</v>
+        <v>178</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>131</v>
+        <v>179</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="8" t="s">
-        <v>132</v>
+        <v>180</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="F2" s="8">
         <v>1</v>
@@ -2461,39 +3103,39 @@
       <c r="K2" s="10">
         <v>0.416666666666667</v>
       </c>
-      <c r="L2" s="29" t="s">
-        <v>133</v>
-      </c>
-      <c r="M2" s="29" t="s">
-        <v>134</v>
+      <c r="L2" s="37" t="s">
+        <v>181</v>
+      </c>
+      <c r="M2" s="37" t="s">
+        <v>182</v>
       </c>
       <c r="N2" s="8">
         <v>17</v>
       </c>
-      <c r="O2" s="29" t="s">
-        <v>134</v>
+      <c r="O2" s="37" t="s">
+        <v>182</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>135</v>
+        <v>183</v>
       </c>
       <c r="Q2" s="15"/>
       <c r="R2" s="2" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>136</v>
+        <v>184</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>137</v>
+        <v>185</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>138</v>
+        <v>186</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>139</v>
+        <v>187</v>
       </c>
       <c r="W2" s="16" t="s">
-        <v>140</v>
+        <v>188</v>
       </c>
       <c r="X2" s="2">
         <v>1</v>

</xml_diff>